<commit_message>
Best AQI file identified, before running RFECV
</commit_message>
<xml_diff>
--- a/code/random_forest-outfiles/date encoding test/date encoding test.xlsx
+++ b/code/random_forest-outfiles/date encoding test/date encoding test.xlsx
@@ -8,24 +8,33 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alex\Documents\GitHub\Research-Spring2021\code\random_forest-outfiles\date encoding test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F79F9D52-90D6-435A-8A8D-AC5CA05C64FE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67ACA2B5-A886-46A5-858F-0ED6B21FE785}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="41">
   <si>
     <t>mean_fit_time</t>
   </si>
@@ -142,6 +151,12 @@
   </si>
   <si>
     <t>['months_from_start']</t>
+  </si>
+  <si>
+    <t>r2_rate</t>
+  </si>
+  <si>
+    <t>test_set_r2_rate</t>
   </si>
 </sst>
 </file>
@@ -157,12 +172,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -177,9 +198,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" quotePrefix="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -195,6 +217,1959 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>R2, train and test sets,</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> percent increase (right to left)</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="stacked"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$X$2:$X$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>9.2802551298081116E-7</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.7848972009629332E-4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>7.0236991471614739E-5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5.2512247815343733E-3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.5914238494205063E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.6287196758256077E-4</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-90D6-4966-A204-B74CBE839093}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$Y$2:$Y$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>-1.1620507089324437E-6</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.9740907776394827E-4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-3.2267019268315459E-4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>6.0003175764099968E-3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.4961526525809241E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2.8876070109961651E-4</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-90D6-4966-A204-B74CBE839093}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="876224911"/>
+        <c:axId val="616859855"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="876224911"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="616859855"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="616859855"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="876224911"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="zero"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" sz="1400" b="0" i="0" baseline="0">
+                <a:effectLst/>
+              </a:rPr>
+              <a:t>R2, train and test sets (right to left)</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US" sz="1100">
+              <a:effectLst/>
+            </a:endParaRPr>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$S$2:$S$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>0.70209771664572995</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.70209706508174097</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.70197177033693803</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.70192246941444003</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.69825577140379502</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.68731763464478501</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.68720570809897297</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-DB1C-490A-9AEA-AD240580ABC2}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$V$2:$V$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>0.713821384686395</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.71382221418400504</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.71360998009794097</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.71384031508995605</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.70958259417819403</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.69912265207438895</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.69892083120515702</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-DB1C-490A-9AEA-AD240580ABC2}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="880375103"/>
+        <c:axId val="880371775"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="880375103"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="880371775"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="880371775"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="880375103"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>166687</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>466725</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>52387</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{919FB21A-2268-4AB0-8A3F-F43F26F0755A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>142875</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>176212</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>447675</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>61912</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2C275308-A875-4481-8310-E3B4F16DAE7B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -460,19 +2435,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Y8"/>
+  <dimension ref="A1:AA8"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
-      <selection activeCell="X10" sqref="X10"/>
+    <sheetView tabSelected="1" topLeftCell="H1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="AA24" sqref="AA24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="24" max="24" width="33.140625" customWidth="1"/>
-    <col min="25" max="25" width="112.28515625" customWidth="1"/>
+    <col min="24" max="24" width="12.42578125" customWidth="1"/>
+    <col min="25" max="25" width="14.140625" customWidth="1"/>
+    <col min="26" max="26" width="35" customWidth="1"/>
+    <col min="27" max="27" width="79.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -542,11 +2519,17 @@
       <c r="W1" t="s">
         <v>22</v>
       </c>
+      <c r="X1" t="s">
+        <v>39</v>
+      </c>
       <c r="Y1" t="s">
+        <v>40</v>
+      </c>
+      <c r="AA1" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>87.503474164009006</v>
       </c>
@@ -616,14 +2599,22 @@
       <c r="W2">
         <v>10</v>
       </c>
-      <c r="X2" s="1" t="s">
+      <c r="X2">
+        <f t="shared" ref="X2:X7" si="0">(S2-S3)/S3</f>
+        <v>9.2802551298081116E-7</v>
+      </c>
+      <c r="Y2">
+        <f t="shared" ref="Y2:Y7" si="1">(V2-V3)/V3</f>
+        <v>-1.1620507089324437E-6</v>
+      </c>
+      <c r="Z2" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="Y2" t="s">
+      <c r="AA2" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="3" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>78.357978010177604</v>
       </c>
@@ -693,14 +2684,22 @@
       <c r="W3">
         <v>10</v>
       </c>
-      <c r="X3" s="1" t="s">
+      <c r="X3">
+        <f t="shared" si="0"/>
+        <v>1.7848972009629332E-4</v>
+      </c>
+      <c r="Y3">
+        <f t="shared" si="1"/>
+        <v>2.9740907776394827E-4</v>
+      </c>
+      <c r="Z3" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="Y3" t="s">
+      <c r="AA3" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="4" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>79.405817937850898</v>
       </c>
@@ -770,14 +2769,22 @@
       <c r="W4">
         <v>9</v>
       </c>
-      <c r="X4" s="1" t="s">
+      <c r="X4">
+        <f t="shared" si="0"/>
+        <v>7.0236991471614739E-5</v>
+      </c>
+      <c r="Y4">
+        <f t="shared" si="1"/>
+        <v>-3.2267019268315459E-4</v>
+      </c>
+      <c r="Z4" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="Y4" t="s">
+      <c r="AA4" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="5" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>80.847213149070697</v>
       </c>
@@ -847,14 +2854,22 @@
       <c r="W5">
         <v>9</v>
       </c>
-      <c r="X5" s="1" t="s">
+      <c r="X5">
+        <f t="shared" si="0"/>
+        <v>5.2512247815343733E-3</v>
+      </c>
+      <c r="Y5">
+        <f t="shared" si="1"/>
+        <v>6.0003175764099968E-3</v>
+      </c>
+      <c r="Z5" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="Y5" t="s">
+      <c r="AA5" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="6" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>81.210599970817498</v>
       </c>
@@ -924,14 +2939,22 @@
       <c r="W6">
         <v>9</v>
       </c>
-      <c r="X6" s="1" t="s">
+      <c r="X6">
+        <f t="shared" si="0"/>
+        <v>1.5914238494205063E-2</v>
+      </c>
+      <c r="Y6">
+        <f t="shared" si="1"/>
+        <v>1.4961526525809241E-2</v>
+      </c>
+      <c r="Z6" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="Y6" t="s">
+      <c r="AA6" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="7" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>80.474527955055194</v>
       </c>
@@ -1001,14 +3024,22 @@
       <c r="W7">
         <v>9</v>
       </c>
-      <c r="X7" s="1" t="s">
+      <c r="X7">
+        <f t="shared" si="0"/>
+        <v>1.6287196758256077E-4</v>
+      </c>
+      <c r="Y7">
+        <f t="shared" si="1"/>
+        <v>2.8876070109961651E-4</v>
+      </c>
+      <c r="Z7" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="Y7" t="s">
+      <c r="AA7" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="8" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>82.280582833290097</v>
       </c>
@@ -1078,10 +3109,10 @@
       <c r="W8">
         <v>8</v>
       </c>
-      <c r="X8" s="1" t="s">
+      <c r="Z8" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="Y8" t="s">
+      <c r="AA8" t="s">
         <v>37</v>
       </c>
     </row>
@@ -1090,5 +3121,6 @@
     <sortCondition descending="1" ref="S1:S8"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>